<commit_message>
Added the correct names
</commit_message>
<xml_diff>
--- a/feedback.xlsx
+++ b/feedback.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -95,8 +95,11 @@
 I am sending you an email</t>
   </si>
   <si>
-    <t xml:space="preserve">The website is working fire_x000D_
+    <t xml:space="preserve">The website is working fire_x005F_x000D_
 </t>
+  </si>
+  <si>
+    <t>nigga you are doing great</t>
   </si>
 </sst>
 </file>
@@ -454,7 +457,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -612,6 +615,17 @@
         <v>26</v>
       </c>
     </row>
+    <row r="20" spans="4:6">
+      <c r="D20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>